<commit_message>
CSI1101 A2: finished password protection, todo choosing password
</commit_message>
<xml_diff>
--- a/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib.xlsx
+++ b/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marty\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Dropbox\Documents\ecu\year_1\sem_2\CSI1101_computer_security\0b_assignment_2_[22MAY15_0900]\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>INTEXT</t>
   </si>
@@ -496,6 +496,30 @@
       </rPr>
       <t>. Boston: Pearson.</t>
     </r>
+  </si>
+  <si>
+    <t>(MITRE, 2014)</t>
+  </si>
+  <si>
+    <t>MITRE. (2014). CVE - CVE-2014-1532. cve.mitre.org. Retrieved March 18, 2015, from http://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2014-1532</t>
+  </si>
+  <si>
+    <t>(SecurityFocus, 2010)</t>
+  </si>
+  <si>
+    <t>SecurityFocus. (2010). Adobe Reader and Acrobat U3D Support Remote Code Execution Vulnerability. Retrieved March 11, 2015, from http://www.securityfocus.com/bid/37756/info</t>
+  </si>
+  <si>
+    <t>(SecurityTracker, 2010)</t>
+  </si>
+  <si>
+    <t>SecurityTracker. (2010). Adobe Acrobat and Adobe Reader Flaws Lets Remote Users Execute Arbitrary Code and Deny Service - SecurityTracker. SecurityTracker. Retrieved March 11, 2015, from http://www.securitytracker.com/id?1023446</t>
+  </si>
+  <si>
+    <t>MITRE. (2006). CVE - CVE-2006-2198. cve.mitre.org. Retrieved March 11, 2015, from http://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2006-2198</t>
+  </si>
+  <si>
+    <t>(MITRE, 2006)</t>
   </si>
 </sst>
 </file>
@@ -830,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,6 +962,38 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CSI1101 A2: finished passwords, user privileges
</commit_message>
<xml_diff>
--- a/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib.xlsx
+++ b/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>INTEXT</t>
   </si>
@@ -520,6 +520,12 @@
   </si>
   <si>
     <t>(MITRE, 2006)</t>
+  </si>
+  <si>
+    <t>(Oliver &amp; Snowden, 2015)</t>
+  </si>
+  <si>
+    <t>Oliver, J., &amp; Snowden, E. [Last Week Tonight]. (2015). Last Week Tonight with John Oliver: Edward Snowden on Passwords. Retrieved May 6, 2015, from https://www.youtube.com/watch?v=yzGzB-yYKcc</t>
   </si>
 </sst>
 </file>
@@ -854,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,6 +1000,14 @@
         <v>30</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CSI1101 A2: started uac section
</commit_message>
<xml_diff>
--- a/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib.xlsx
+++ b/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>INTEXT</t>
   </si>
@@ -501,31 +501,259 @@
     <t>(MITRE, 2014)</t>
   </si>
   <si>
-    <t>MITRE. (2014). CVE - CVE-2014-1532. cve.mitre.org. Retrieved March 18, 2015, from http://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2014-1532</t>
-  </si>
-  <si>
     <t>(SecurityFocus, 2010)</t>
   </si>
   <si>
-    <t>SecurityFocus. (2010). Adobe Reader and Acrobat U3D Support Remote Code Execution Vulnerability. Retrieved March 11, 2015, from http://www.securityfocus.com/bid/37756/info</t>
-  </si>
-  <si>
     <t>(SecurityTracker, 2010)</t>
   </si>
   <si>
-    <t>SecurityTracker. (2010). Adobe Acrobat and Adobe Reader Flaws Lets Remote Users Execute Arbitrary Code and Deny Service - SecurityTracker. SecurityTracker. Retrieved March 11, 2015, from http://www.securitytracker.com/id?1023446</t>
-  </si>
-  <si>
-    <t>MITRE. (2006). CVE - CVE-2006-2198. cve.mitre.org. Retrieved March 11, 2015, from http://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2006-2198</t>
-  </si>
-  <si>
     <t>(MITRE, 2006)</t>
   </si>
   <si>
     <t>(Oliver &amp; Snowden, 2015)</t>
   </si>
   <si>
-    <t>Oliver, J., &amp; Snowden, E. [Last Week Tonight]. (2015). Last Week Tonight with John Oliver: Edward Snowden on Passwords. Retrieved May 6, 2015, from https://www.youtube.com/watch?v=yzGzB-yYKcc</t>
+    <t>(Goodin, 2014)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Goodin, D. (2014). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stanford’s password policy shuns one-size-fits-all security | Ars Technica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ars Technica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved April 30, 2015, from http://arstechnica.com/security/2014/04/25/stanfords-password-policy-shuns-one-size-fits-all-security/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MITRE. (2014). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CVE - CVE-2014-1532</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cve.mitre.org</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved March 18, 2015, from http://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2014-1532</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SecurityFocus. (2010). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Adobe Reader and Acrobat U3D Support Remote Code Execution Vulnerability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved March 11, 2015, from http://www.securityfocus.com/bid/37756/info</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SecurityTracker. (2010). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Adobe Acrobat and Adobe Reader Flaws Lets Remote Users Execute Arbitrary Code and Deny Service - SecurityTracker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SecurityTracker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved March 11, 2015, from http://www.securitytracker.com/id?1023446</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MITRE. (2006). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CVE - CVE-2006-2198</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cve.mitre.org</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved March 11, 2015, from http://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2006-2198</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Oliver, J., &amp; Snowden, E. (2015). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Last Week Tonight with John Oliver: Edward Snowden on Passwords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 6, 2015, from https://www.youtube.com/watch?v=yzGzB-yYKcc</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -860,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,40 +1200,48 @@
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CSI1101 A2: finished uac, summary
</commit_message>
<xml_diff>
--- a/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib.xlsx
+++ b/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>INTEXT</t>
   </si>
@@ -754,6 +754,85 @@
       </rPr>
       <t>. Retrieved May 6, 2015, from https://www.youtube.com/watch?v=yzGzB-yYKcc</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microsoft. (n.d.-a). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Internet Explorer system requirements IE11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microsoft</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved April 19, 2015, from http://windows.microsoft.com/en-au/internet-explorer/ie-system-requirements#ie=ie-11</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microsoft. (n.d.-b). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What is User Account Control? - Windows Help</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved March 14, 2015, from http://windows.microsoft.com/en-au/windows/what-is-user-account-control#1TC=windows-vista</t>
+    </r>
+  </si>
+  <si>
+    <t>(Microsoft, n.d.-b)</t>
+  </si>
+  <si>
+    <t>(Microsoft, n.d.-a)</t>
   </si>
 </sst>
 </file>
@@ -1088,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,141 +1189,160 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B20">
+    <sortCondition ref="B20"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>